<commit_message>
?FieldReduction is supported now
The ?FieldReduction allows reducing and/or renaming fields
</commit_message>
<xml_diff>
--- a/src/Data Loader/Data Loader Configuration.xlsx
+++ b/src/Data Loader/Data Loader Configuration.xlsx
@@ -16,6 +16,7 @@
     <sheet name="Data Sources" sheetId="1" r:id="rId2"/>
     <sheet name="Tables" sheetId="2" r:id="rId3"/>
     <sheet name="Description" sheetId="4" r:id="rId4"/>
+    <sheet name="TABLE2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="86">
   <si>
     <t>Data Connection</t>
   </si>
@@ -192,33 +193,6 @@
   </si>
   <si>
     <t>TABLES</t>
-  </si>
-  <si>
-    <r>
-      <t>Редукция и/или переименование поле (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>пока не реализовано</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -571,6 +545,32 @@
   </si>
   <si>
     <t>Название очереди&gt; указнной в имени приложения по шаблону ИМЯ.LOADER.ОЧЕРЕДЬ</t>
+  </si>
+  <si>
+    <t>Редукция и/или переименование поле - задаёт имя листа в файле конфигурации с перечнем полей в составе пары OriginalFieldName + NewFieldName "оригинальное имя поля + новое имя поля", при отсутствии нового имени поля используется оригинальное, т.е. поле не переименовывается.
+Необходимость включения поля определяется атрибутом ?Active - Активность (1/0).
+В OriginalFieldName и NewFieldName не допускается наличие двойных кавычек, при наличии они будут вырезаны</t>
+  </si>
+  <si>
+    <t>OriginalFieldName</t>
+  </si>
+  <si>
+    <t>NewFieldName</t>
+  </si>
+  <si>
+    <t>FIELD1</t>
+  </si>
+  <si>
+    <t>FIELD2</t>
+  </si>
+  <si>
+    <t>FIELD3</t>
+  </si>
+  <si>
+    <t>Field No. 1</t>
+  </si>
+  <si>
+    <t>Field No. 3</t>
   </si>
 </sst>
 </file>
@@ -660,7 +660,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -687,12 +687,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -732,7 +726,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -770,13 +764,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1082,6 +1073,18 @@
     <tableColumn id="12" name="Select" dataDxfId="2"/>
     <tableColumn id="13" name="Queue" dataDxfId="1"/>
     <tableColumn id="14" name="Comments" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Таблица3" displayName="Таблица3" ref="A1:C4" totalsRowShown="0">
+  <autoFilter ref="A1:C4"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OriginalFieldName"/>
+    <tableColumn id="2" name="NewFieldName"/>
+    <tableColumn id="3" name="?Active"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1511,16 +1514,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
         <v>67</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>68</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>69</v>
-      </c>
-      <c r="D2" t="s">
-        <v>70</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1539,7 +1542,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1593,7 +1596,7 @@
       <c r="J1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="8" t="s">
         <v>24</v>
       </c>
       <c r="L1" s="8" t="s">
@@ -1614,13 +1617,13 @@
     </row>
     <row r="2" spans="1:16" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2" s="11">
         <v>0</v>
@@ -1635,13 +1638,13 @@
         <v>12</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L2" s="11">
         <v>0</v>
@@ -1650,13 +1653,10 @@
     </row>
     <row r="3" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3" s="11">
         <v>0</v>
@@ -1673,6 +1673,9 @@
       <c r="H3" s="12"/>
       <c r="I3" s="11" t="s">
         <v>11</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="L3" s="11">
         <v>1</v>
@@ -1695,8 +1698,8 @@
   </sheetPr>
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1712,15 +1715,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -1728,7 +1731,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -1736,7 +1739,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -1744,7 +1747,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>32</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -1752,7 +1755,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -1760,7 +1763,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -1768,7 +1771,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -1776,23 +1779,23 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="14"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -1800,15 +1803,15 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -1816,7 +1819,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -1824,7 +1827,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -1832,103 +1835,103 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="14"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="13"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="15" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="9" t="s">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="9" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="9" t="s">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="9" t="s">
+    <row r="23" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B23" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="16" t="s">
+    <row r="27" spans="2:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="B27" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C28" s="9" t="s">
@@ -1936,31 +1939,31 @@
       </c>
     </row>
     <row r="29" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B30" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="9" t="s">
+    <row r="31" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B31" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C32" s="9" t="s">
@@ -1968,9 +1971,73 @@
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="16"/>
+      <c r="B33" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Amendments to the variables
</commit_message>
<xml_diff>
--- a/src/Data Loader/Data Loader Configuration.xlsx
+++ b/src/Data Loader/Data Loader Configuration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="3" r:id="rId1"/>
@@ -96,9 +96,6 @@
     <t>sReloadMode</t>
   </si>
   <si>
-    <t>Режим загрузки: 'F' - Full loads, 'R' - Partial load</t>
-  </si>
-  <si>
     <t>LoadAndStoreField</t>
   </si>
   <si>
@@ -571,6 +568,9 @@
   </si>
   <si>
     <t>Field No. 3</t>
+  </si>
+  <si>
+    <t>Режим частичной загрузки (LoadMode=P): 'F' - Full load с даты sFullExtract_StartDate, 'R' - Partial load с даты sPartialExtract_StartDate</t>
   </si>
 </sst>
 </file>
@@ -1355,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,28 +1373,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1408,7 +1408,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2" s="6">
         <v>1</v>
@@ -1432,7 +1432,7 @@
         <v>19</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="6">
         <v>1</v>
@@ -1445,7 +1445,7 @@
       </c>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="6">
         <v>1</v>
@@ -1465,7 +1465,7 @@
         <v>17</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="H4" s="7"/>
     </row>
@@ -1506,24 +1506,24 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
         <v>66</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>67</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>68</v>
-      </c>
-      <c r="D2" t="s">
-        <v>69</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1541,7 +1541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -1579,10 +1579,10 @@
         <v>9</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>10</v>
@@ -1594,13 +1594,13 @@
         <v>14</v>
       </c>
       <c r="J1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>5</v>
@@ -1609,21 +1609,21 @@
         <v>6</v>
       </c>
       <c r="O1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D2" s="11">
         <v>0</v>
@@ -1632,19 +1632,19 @@
         <v>1</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L2" s="11">
         <v>0</v>
@@ -1653,10 +1653,10 @@
     </row>
     <row r="3" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" s="11">
         <v>0</v>
@@ -1665,7 +1665,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>11</v>
@@ -1675,7 +1675,7 @@
         <v>11</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L3" s="11">
         <v>1</v>
@@ -1716,7 +1716,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="14"/>
@@ -1724,71 +1724,71 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="14"/>
@@ -1799,7 +1799,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1807,7 +1807,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1815,7 +1815,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1823,20 +1823,20 @@
         <v>0</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" s="13"/>
       <c r="C16" s="14"/>
@@ -1847,7 +1847,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -1855,7 +1855,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -1863,7 +1863,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -1871,23 +1871,23 @@
         <v>9</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="60" x14ac:dyDescent="0.25">
@@ -1895,7 +1895,7 @@
         <v>10</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -1903,7 +1903,7 @@
         <v>4</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1911,31 +1911,31 @@
         <v>14</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="105" x14ac:dyDescent="0.25">
       <c r="B27" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -1943,7 +1943,7 @@
         <v>5</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -1951,23 +1951,23 @@
         <v>6</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
@@ -1995,21 +1995,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
         <v>79</v>
       </c>
-      <c r="B1" t="s">
-        <v>80</v>
-      </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2017,7 +2017,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2025,10 +2025,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4">
         <v>1</v>

</xml_diff>